<commit_message>
Finalisation of v0.3.0 PCB
</commit_message>
<xml_diff>
--- a/KiCad/FairberryMainboard/cpl/CPL.xlsx
+++ b/KiCad/FairberryMainboard/cpl/CPL.xlsx
@@ -163,7 +163,7 @@
     <t xml:space="preserve">-88.200000</t>
   </si>
   <si>
-    <t xml:space="preserve">135.000000</t>
+    <t xml:space="preserve">45.000000</t>
   </si>
   <si>
     <t xml:space="preserve">U2</t>
@@ -293,10 +293,10 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.74"/>

</xml_diff>